<commit_message>
Modif photo + un peu de front
</commit_message>
<xml_diff>
--- a/Suivi.xlsx
+++ b/Suivi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\ENI\Projet PHP Symfony\projetSortir.com\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\ENI\Logiciels\wamp64\www\Sortir.com\sorties.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -417,6 +417,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -431,9 +434,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -810,11 +810,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="12895672"/>
-        <c:axId val="12896456"/>
+        <c:axId val="430584744"/>
+        <c:axId val="430586312"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="12896456"/>
+        <c:axId val="430586312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,12 +837,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="12895672"/>
+        <c:crossAx val="430584744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="12895672"/>
+        <c:axId val="430584744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -887,7 +887,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12896456"/>
+        <c:crossAx val="430586312"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1310,12 +1310,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
@@ -1404,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J87" sqref="J87"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,24 +1452,24 @@
       <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:16" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="12"/>
@@ -1605,7 +1605,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="26">
         <v>0</v>
       </c>
       <c r="B8" s="18" t="s">
@@ -1626,7 +1626,7 @@
       <c r="O8" s="19"/>
     </row>
     <row r="9" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -1643,7 +1643,7 @@
       <c r="O9" s="19"/>
     </row>
     <row r="10" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="20"/>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -1660,7 +1660,7 @@
       <c r="O10" s="19"/>
     </row>
     <row r="11" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -1677,7 +1677,7 @@
       <c r="O11" s="19"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="21"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
@@ -1694,7 +1694,7 @@
       <c r="O12" s="19"/>
     </row>
     <row r="13" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="21"/>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -1711,7 +1711,7 @@
       <c r="O13" s="19"/>
     </row>
     <row r="14" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="21"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -1728,7 +1728,7 @@
       <c r="O14" s="19"/>
     </row>
     <row r="15" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="26">
+      <c r="A15" s="27">
         <v>1</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -1778,7 +1778,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="21" t="s">
         <v>30</v>
       </c>
@@ -1801,7 +1801,7 @@
       <c r="O16" s="19"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="21" t="s">
         <v>31</v>
       </c>
@@ -1824,7 +1824,7 @@
       <c r="O17" s="19"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="21" t="s">
         <v>32</v>
       </c>
@@ -1847,7 +1847,7 @@
       <c r="O18" s="19"/>
     </row>
     <row r="19" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="18" t="s">
         <v>33</v>
       </c>
@@ -1870,7 +1870,7 @@
       <c r="O19" s="19"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="21" t="s">
         <v>34</v>
       </c>
@@ -1893,7 +1893,7 @@
       <c r="O20" s="19"/>
     </row>
     <row r="21" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="15" t="s">
         <v>39</v>
       </c>
@@ -1943,7 +1943,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="18" t="s">
         <v>30</v>
       </c>
@@ -1966,7 +1966,7 @@
       <c r="O22" s="19"/>
     </row>
     <row r="23" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="18" t="s">
         <v>31</v>
       </c>
@@ -1989,7 +1989,7 @@
       <c r="O23" s="19"/>
     </row>
     <row r="24" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="18" t="s">
         <v>32</v>
       </c>
@@ -2012,7 +2012,7 @@
       <c r="O24" s="19"/>
     </row>
     <row r="25" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="18" t="s">
         <v>33</v>
       </c>
@@ -2035,7 +2035,7 @@
       <c r="O25" s="19"/>
     </row>
     <row r="26" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="20" t="s">
         <v>34</v>
       </c>
@@ -2058,7 +2058,7 @@
       <c r="O26" s="19"/>
     </row>
     <row r="27" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="15" t="s">
         <v>40</v>
       </c>
@@ -2107,7 +2107,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="18" t="s">
         <v>30</v>
       </c>
@@ -2130,7 +2130,7 @@
       <c r="O28" s="19"/>
     </row>
     <row r="29" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="18" t="s">
         <v>31</v>
       </c>
@@ -2153,7 +2153,7 @@
       <c r="O29" s="19"/>
     </row>
     <row r="30" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="18" t="s">
         <v>32</v>
       </c>
@@ -2176,7 +2176,7 @@
       <c r="O30" s="19"/>
     </row>
     <row r="31" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="18" t="s">
         <v>33</v>
       </c>
@@ -2199,7 +2199,7 @@
       <c r="O31" s="19"/>
     </row>
     <row r="32" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="20" t="s">
         <v>34</v>
       </c>
@@ -2222,8 +2222,8 @@
       <c r="O32" s="19"/>
     </row>
     <row r="33" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
-      <c r="B33" s="28" t="s">
+      <c r="A33" s="27"/>
+      <c r="B33" s="23" t="s">
         <v>42</v>
       </c>
       <c r="C33" s="16"/>
@@ -2272,7 +2272,7 @@
       </c>
     </row>
     <row r="34" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="18" t="s">
         <v>30</v>
       </c>
@@ -2295,7 +2295,7 @@
       <c r="O34" s="19"/>
     </row>
     <row r="35" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="18" t="s">
         <v>31</v>
       </c>
@@ -2318,7 +2318,7 @@
       <c r="O35" s="19"/>
     </row>
     <row r="36" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="18" t="s">
         <v>32</v>
       </c>
@@ -2341,7 +2341,7 @@
       <c r="O36" s="19"/>
     </row>
     <row r="37" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="18" t="s">
         <v>33</v>
       </c>
@@ -2364,7 +2364,7 @@
       <c r="O37" s="19"/>
     </row>
     <row r="38" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="A38" s="27"/>
       <c r="B38" s="20" t="s">
         <v>34</v>
       </c>
@@ -2387,8 +2387,8 @@
       <c r="O38" s="19"/>
     </row>
     <row r="39" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="26"/>
-      <c r="B39" s="28" t="s">
+      <c r="A39" s="27"/>
+      <c r="B39" s="23" t="s">
         <v>43</v>
       </c>
       <c r="C39" s="16"/>
@@ -2437,7 +2437,7 @@
       </c>
     </row>
     <row r="40" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="18" t="s">
         <v>30</v>
       </c>
@@ -2460,7 +2460,7 @@
       <c r="O40" s="19"/>
     </row>
     <row r="41" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="A41" s="27"/>
       <c r="B41" s="18" t="s">
         <v>31</v>
       </c>
@@ -2483,7 +2483,7 @@
       <c r="O41" s="19"/>
     </row>
     <row r="42" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="18" t="s">
         <v>32</v>
       </c>
@@ -2506,7 +2506,7 @@
       <c r="O42" s="19"/>
     </row>
     <row r="43" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+      <c r="A43" s="27"/>
       <c r="B43" s="18" t="s">
         <v>33</v>
       </c>
@@ -2529,7 +2529,7 @@
       <c r="O43" s="19"/>
     </row>
     <row r="44" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="20" t="s">
         <v>34</v>
       </c>
@@ -2552,7 +2552,7 @@
       <c r="O44" s="19"/>
     </row>
     <row r="45" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="27">
+      <c r="A45" s="28">
         <v>2</v>
       </c>
       <c r="B45" s="15" t="s">
@@ -2580,28 +2580,27 @@
         <v>1</v>
       </c>
       <c r="K45" s="17">
-        <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L45" s="17">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45" s="17">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45" s="17">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O45" s="17">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
+      <c r="A46" s="28"/>
       <c r="B46" s="21" t="s">
         <v>30</v>
       </c>
@@ -2624,7 +2623,7 @@
       <c r="O46" s="19"/>
     </row>
     <row r="47" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
+      <c r="A47" s="28"/>
       <c r="B47" s="21" t="s">
         <v>31</v>
       </c>
@@ -2647,7 +2646,7 @@
       <c r="O47" s="19"/>
     </row>
     <row r="48" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="27"/>
+      <c r="A48" s="28"/>
       <c r="B48" s="21" t="s">
         <v>32</v>
       </c>
@@ -2670,7 +2669,7 @@
       <c r="O48" s="19"/>
     </row>
     <row r="49" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="18" t="s">
         <v>33</v>
       </c>
@@ -2678,7 +2677,7 @@
         <v>4</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E49" s="19"/>
       <c r="F49" s="19"/>
@@ -2693,7 +2692,7 @@
       <c r="O49" s="19"/>
     </row>
     <row r="50" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="27"/>
+      <c r="A50" s="28"/>
       <c r="B50" s="18" t="s">
         <v>34</v>
       </c>
@@ -2716,7 +2715,7 @@
       <c r="O50" s="19"/>
     </row>
     <row r="51" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="27"/>
+      <c r="A51" s="28"/>
       <c r="B51" s="15" t="s">
         <v>35</v>
       </c>
@@ -2742,28 +2741,27 @@
         <v>8</v>
       </c>
       <c r="K51" s="17">
-        <f t="shared" si="15"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L51" s="17">
         <f t="shared" si="15"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M51" s="17">
         <f t="shared" si="15"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N51" s="17">
         <f t="shared" si="15"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O51" s="17">
         <f t="shared" si="15"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
+      <c r="A52" s="28"/>
       <c r="B52" s="21" t="s">
         <v>30</v>
       </c>
@@ -2771,7 +2769,7 @@
         <v>3</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E52" s="19"/>
       <c r="F52" s="19"/>
@@ -2786,7 +2784,7 @@
       <c r="O52" s="19"/>
     </row>
     <row r="53" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="27"/>
+      <c r="A53" s="28"/>
       <c r="B53" s="21" t="s">
         <v>31</v>
       </c>
@@ -2794,7 +2792,7 @@
         <v>3</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E53" s="19"/>
       <c r="F53" s="19"/>
@@ -2809,7 +2807,7 @@
       <c r="O53" s="19"/>
     </row>
     <row r="54" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="27"/>
+      <c r="A54" s="28"/>
       <c r="B54" s="21" t="s">
         <v>32</v>
       </c>
@@ -2817,7 +2815,7 @@
         <v>3</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E54" s="19"/>
       <c r="F54" s="19"/>
@@ -2832,7 +2830,7 @@
       <c r="O54" s="19"/>
     </row>
     <row r="55" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="27"/>
+      <c r="A55" s="28"/>
       <c r="B55" s="18" t="s">
         <v>33</v>
       </c>
@@ -2840,7 +2838,7 @@
         <v>3</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E55" s="19"/>
       <c r="F55" s="19"/>
@@ -2855,7 +2853,7 @@
       <c r="O55" s="19"/>
     </row>
     <row r="56" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="27"/>
+      <c r="A56" s="28"/>
       <c r="B56" s="18" t="s">
         <v>34</v>
       </c>
@@ -2863,7 +2861,7 @@
         <v>3</v>
       </c>
       <c r="D56" s="19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E56" s="19"/>
       <c r="F56" s="19"/>
@@ -2878,7 +2876,7 @@
       <c r="O56" s="19"/>
     </row>
     <row r="57" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="27"/>
+      <c r="A57" s="28"/>
       <c r="B57" s="15" t="s">
         <v>46</v>
       </c>
@@ -2928,7 +2926,7 @@
       </c>
     </row>
     <row r="58" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="27"/>
+      <c r="A58" s="28"/>
       <c r="B58" s="21" t="s">
         <v>30</v>
       </c>
@@ -2951,7 +2949,7 @@
       <c r="O58" s="19"/>
     </row>
     <row r="59" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="27"/>
+      <c r="A59" s="28"/>
       <c r="B59" s="21" t="s">
         <v>31</v>
       </c>
@@ -2974,7 +2972,7 @@
       <c r="O59" s="19"/>
     </row>
     <row r="60" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="27"/>
+      <c r="A60" s="28"/>
       <c r="B60" s="21" t="s">
         <v>32</v>
       </c>
@@ -2997,7 +2995,7 @@
       <c r="O60" s="19"/>
     </row>
     <row r="61" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="27"/>
+      <c r="A61" s="28"/>
       <c r="B61" s="18" t="s">
         <v>33</v>
       </c>
@@ -3020,7 +3018,7 @@
       <c r="O61" s="19"/>
     </row>
     <row r="62" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="27"/>
+      <c r="A62" s="28"/>
       <c r="B62" s="18" t="s">
         <v>34</v>
       </c>
@@ -3043,7 +3041,7 @@
       <c r="O62" s="19"/>
     </row>
     <row r="63" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="27"/>
+      <c r="A63" s="28"/>
       <c r="B63" s="15" t="s">
         <v>47</v>
       </c>
@@ -3093,7 +3091,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="27"/>
+      <c r="A64" s="28"/>
       <c r="B64" s="21" t="s">
         <v>30</v>
       </c>
@@ -3116,7 +3114,7 @@
       <c r="O64" s="19"/>
     </row>
     <row r="65" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="27"/>
+      <c r="A65" s="28"/>
       <c r="B65" s="21" t="s">
         <v>31</v>
       </c>
@@ -3139,7 +3137,7 @@
       <c r="O65" s="19"/>
     </row>
     <row r="66" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="27"/>
+      <c r="A66" s="28"/>
       <c r="B66" s="21" t="s">
         <v>32</v>
       </c>
@@ -3162,7 +3160,7 @@
       <c r="O66" s="19"/>
     </row>
     <row r="67" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="27"/>
+      <c r="A67" s="28"/>
       <c r="B67" s="18" t="s">
         <v>33</v>
       </c>
@@ -3185,7 +3183,7 @@
       <c r="O67" s="19"/>
     </row>
     <row r="68" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="27"/>
+      <c r="A68" s="28"/>
       <c r="B68" s="18" t="s">
         <v>34</v>
       </c>
@@ -3208,7 +3206,7 @@
       <c r="O68" s="19"/>
     </row>
     <row r="69" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="27"/>
+      <c r="A69" s="28"/>
       <c r="B69" s="15"/>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
@@ -3257,7 +3255,7 @@
       </c>
     </row>
     <row r="70" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="27"/>
+      <c r="A70" s="28"/>
       <c r="B70" s="18"/>
       <c r="C70" s="19"/>
       <c r="D70" s="19"/>
@@ -3274,7 +3272,7 @@
       <c r="O70" s="19"/>
     </row>
     <row r="71" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="27"/>
+      <c r="A71" s="28"/>
       <c r="B71" s="18"/>
       <c r="C71" s="19"/>
       <c r="D71" s="19"/>
@@ -3291,7 +3289,7 @@
       <c r="O71" s="19"/>
     </row>
     <row r="72" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="27"/>
+      <c r="A72" s="28"/>
       <c r="B72" s="18"/>
       <c r="C72" s="19"/>
       <c r="D72" s="19"/>
@@ -3308,7 +3306,7 @@
       <c r="O72" s="19"/>
     </row>
     <row r="73" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="27"/>
+      <c r="A73" s="28"/>
       <c r="B73" s="18"/>
       <c r="C73" s="19"/>
       <c r="D73" s="19"/>
@@ -3325,7 +3323,7 @@
       <c r="O73" s="19"/>
     </row>
     <row r="74" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="27"/>
+      <c r="A74" s="28"/>
       <c r="B74" s="18"/>
       <c r="C74" s="19"/>
       <c r="D74" s="19"/>
@@ -3342,7 +3340,7 @@
       <c r="O74" s="19"/>
     </row>
     <row r="75" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="27"/>
+      <c r="A75" s="28"/>
       <c r="B75" s="15" t="s">
         <v>44</v>
       </c>
@@ -3392,7 +3390,7 @@
       </c>
     </row>
     <row r="76" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="27"/>
+      <c r="A76" s="28"/>
       <c r="B76" s="21" t="s">
         <v>30</v>
       </c>
@@ -3415,7 +3413,7 @@
       <c r="O76" s="19"/>
     </row>
     <row r="77" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="27"/>
+      <c r="A77" s="28"/>
       <c r="B77" s="21" t="s">
         <v>31</v>
       </c>
@@ -3438,7 +3436,7 @@
       <c r="O77" s="19"/>
     </row>
     <row r="78" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="27"/>
+      <c r="A78" s="28"/>
       <c r="B78" s="21" t="s">
         <v>32</v>
       </c>
@@ -3461,7 +3459,7 @@
       <c r="O78" s="19"/>
     </row>
     <row r="79" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="27"/>
+      <c r="A79" s="28"/>
       <c r="B79" s="18" t="s">
         <v>33</v>
       </c>
@@ -3484,7 +3482,7 @@
       <c r="O79" s="19"/>
     </row>
     <row r="80" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="27"/>
+      <c r="A80" s="28"/>
       <c r="B80" s="18" t="s">
         <v>34</v>
       </c>
@@ -3507,7 +3505,7 @@
       <c r="O80" s="19"/>
     </row>
     <row r="81" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A81" s="27"/>
+      <c r="A81" s="28"/>
       <c r="B81" s="15" t="s">
         <v>45</v>
       </c>
@@ -3557,7 +3555,7 @@
       </c>
     </row>
     <row r="82" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="27"/>
+      <c r="A82" s="28"/>
       <c r="B82" s="21" t="s">
         <v>30</v>
       </c>
@@ -3580,7 +3578,7 @@
       <c r="O82" s="19"/>
     </row>
     <row r="83" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="27"/>
+      <c r="A83" s="28"/>
       <c r="B83" s="21" t="s">
         <v>31</v>
       </c>
@@ -3603,7 +3601,7 @@
       <c r="O83" s="19"/>
     </row>
     <row r="84" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="27"/>
+      <c r="A84" s="28"/>
       <c r="B84" s="21" t="s">
         <v>32</v>
       </c>
@@ -3626,7 +3624,7 @@
       <c r="O84" s="19"/>
     </row>
     <row r="85" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="27"/>
+      <c r="A85" s="28"/>
       <c r="B85" s="18" t="s">
         <v>33</v>
       </c>
@@ -3649,7 +3647,7 @@
       <c r="O85" s="19"/>
     </row>
     <row r="86" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="27"/>
+      <c r="A86" s="28"/>
       <c r="B86" s="18" t="s">
         <v>34</v>
       </c>
@@ -3672,7 +3670,7 @@
       <c r="O86" s="19"/>
     </row>
     <row r="87" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A87" s="27"/>
+      <c r="A87" s="28"/>
       <c r="B87" s="15" t="s">
         <v>48</v>
       </c>
@@ -3722,7 +3720,7 @@
       </c>
     </row>
     <row r="88" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="27"/>
+      <c r="A88" s="28"/>
       <c r="B88" s="21" t="s">
         <v>30</v>
       </c>
@@ -3745,7 +3743,7 @@
       <c r="O88" s="19"/>
     </row>
     <row r="89" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="27"/>
+      <c r="A89" s="28"/>
       <c r="B89" s="21" t="s">
         <v>31</v>
       </c>
@@ -3768,7 +3766,7 @@
       <c r="O89" s="19"/>
     </row>
     <row r="90" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="27"/>
+      <c r="A90" s="28"/>
       <c r="B90" s="21" t="s">
         <v>32</v>
       </c>
@@ -3791,7 +3789,7 @@
       <c r="O90" s="19"/>
     </row>
     <row r="91" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="27"/>
+      <c r="A91" s="28"/>
       <c r="B91" s="18" t="s">
         <v>33</v>
       </c>
@@ -3814,7 +3812,7 @@
       <c r="O91" s="19"/>
     </row>
     <row r="92" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="27"/>
+      <c r="A92" s="28"/>
       <c r="B92" s="18" t="s">
         <v>34</v>
       </c>
@@ -3837,7 +3835,7 @@
       <c r="O92" s="19"/>
     </row>
     <row r="93" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="27"/>
+      <c r="A93" s="28"/>
       <c r="B93" s="18"/>
       <c r="C93" s="19"/>
       <c r="D93" s="19"/>
@@ -3854,7 +3852,7 @@
       <c r="O93" s="19"/>
     </row>
     <row r="94" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="27"/>
+      <c r="A94" s="28"/>
       <c r="B94" s="18"/>
       <c r="C94" s="19"/>
       <c r="D94" s="19"/>
@@ -3902,23 +3900,23 @@
       </c>
       <c r="K95" s="22">
         <f t="shared" si="62"/>
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="L95" s="22">
         <f t="shared" si="62"/>
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="M95" s="22">
         <f t="shared" si="62"/>
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="N95" s="22">
         <f t="shared" si="62"/>
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="O95" s="22">
         <f t="shared" si="62"/>
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Page Campus (Suppr at Ajout)
</commit_message>
<xml_diff>
--- a/Suivi.xlsx
+++ b/Suivi.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="51">
   <si>
     <t>Paramètres à renseigner avant d'exploiter l'onglet de suivi</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>2006 - Annuler une sortie</t>
+  </si>
+  <si>
+    <t>Clôture des inscriptions</t>
   </si>
 </sst>
 </file>
@@ -813,11 +816,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="361204152"/>
-        <c:axId val="361207680"/>
+        <c:axId val="307206032"/>
+        <c:axId val="307206816"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="361207680"/>
+        <c:axId val="307206816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -840,12 +843,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="361204152"/>
+        <c:crossAx val="307206032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="361204152"/>
+        <c:axId val="307206032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -890,7 +893,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361207680"/>
+        <c:crossAx val="307206816"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1407,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K97" sqref="K97"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70:B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3208,7 +3211,9 @@
     </row>
     <row r="69" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="28"/>
-      <c r="B69" s="15"/>
+      <c r="B69" s="15" t="s">
+        <v>50</v>
+      </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
       <c r="E69" s="17">
@@ -3257,8 +3262,12 @@
     </row>
     <row r="70" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="28"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="19"/>
+      <c r="B70" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="D70" s="19"/>
       <c r="E70" s="19"/>
       <c r="F70" s="19"/>
@@ -3274,8 +3283,12 @@
     </row>
     <row r="71" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="28"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="19"/>
+      <c r="B71" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="D71" s="19"/>
       <c r="E71" s="19"/>
       <c r="F71" s="19"/>
@@ -3291,8 +3304,12 @@
     </row>
     <row r="72" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="28"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="19"/>
+      <c r="B72" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="D72" s="19"/>
       <c r="E72" s="19"/>
       <c r="F72" s="19"/>
@@ -3308,8 +3325,12 @@
     </row>
     <row r="73" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="28"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="19"/>
+      <c r="B73" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="D73" s="19"/>
       <c r="E73" s="19"/>
       <c r="F73" s="19"/>
@@ -3325,8 +3346,12 @@
     </row>
     <row r="74" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="28"/>
-      <c r="B74" s="18"/>
-      <c r="C74" s="19"/>
+      <c r="B74" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="D74" s="19"/>
       <c r="E74" s="19"/>
       <c r="F74" s="19"/>

</xml_diff>

<commit_message>
Icon + Suppression dynamique avec Pop up
</commit_message>
<xml_diff>
--- a/Suivi.xlsx
+++ b/Suivi.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="52">
   <si>
     <t>Paramètres à renseigner avant d'exploiter l'onglet de suivi</t>
   </si>
@@ -184,7 +184,10 @@
     <t>2006 - Annuler une sortie</t>
   </si>
   <si>
-    <t>Clôture des inscriptions</t>
+    <t>1007 - Inscrire un utilisateur manuellement</t>
+  </si>
+  <si>
+    <t>2005 - Clôture des inscriptions</t>
   </si>
 </sst>
 </file>
@@ -816,11 +819,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="307206032"/>
-        <c:axId val="307206816"/>
+        <c:axId val="210912000"/>
+        <c:axId val="210911608"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="307206816"/>
+        <c:axId val="210911608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,12 +846,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="307206032"/>
+        <c:crossAx val="210912000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="307206032"/>
+        <c:axId val="210912000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -893,7 +896,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="307206816"/>
+        <c:crossAx val="210911608"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1408,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P108"/>
+  <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:B74"/>
+    <sheetView tabSelected="1" topLeftCell="F96" workbookViewId="0">
+      <selection activeCell="J117" sqref="J117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,16 +2102,15 @@
         <v>7</v>
       </c>
       <c r="M27" s="17">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N27" s="17">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O27" s="17">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2189,7 +2191,7 @@
         <v>5</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
@@ -2556,60 +2558,61 @@
       <c r="O44" s="19"/>
     </row>
     <row r="45" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="28">
-        <v>2</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>41</v>
+      <c r="A45" s="27"/>
+      <c r="B45" s="23" t="s">
+        <v>50</v>
       </c>
       <c r="C45" s="16"/>
       <c r="D45" s="16"/>
       <c r="E45" s="17">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F45" s="17">
-        <v>22</v>
+        <f t="shared" ref="F45" si="14">E45</f>
+        <v>6</v>
       </c>
       <c r="G45" s="17">
-        <v>14</v>
+        <f t="shared" ref="G45" si="15">F45</f>
+        <v>6</v>
       </c>
       <c r="H45" s="17">
+        <f t="shared" ref="H45" si="16">G45</f>
         <v>6</v>
       </c>
       <c r="I45" s="17">
         <v>1</v>
       </c>
       <c r="J45" s="17">
-        <f t="shared" ref="J45:O45" si="14">I45</f>
+        <f t="shared" ref="J45" si="17">I45</f>
         <v>1</v>
       </c>
       <c r="K45" s="17">
-        <v>0</v>
+        <f t="shared" ref="K45" si="18">J45</f>
+        <v>1</v>
       </c>
       <c r="L45" s="17">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" ref="L45" si="19">K45</f>
+        <v>1</v>
       </c>
       <c r="M45" s="17">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" ref="M45" si="20">L45</f>
+        <v>1</v>
       </c>
       <c r="N45" s="17">
-        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O45" s="17">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="O45" si="21">N45</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
-      <c r="B46" s="21" t="s">
+      <c r="A46" s="27"/>
+      <c r="B46" s="18" t="s">
         <v>30</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D46" s="19" t="s">
         <v>11</v>
@@ -2627,12 +2630,12 @@
       <c r="O46" s="19"/>
     </row>
     <row r="47" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="28"/>
-      <c r="B47" s="21" t="s">
+      <c r="A47" s="27"/>
+      <c r="B47" s="18" t="s">
         <v>31</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D47" s="19" t="s">
         <v>11</v>
@@ -2650,12 +2653,12 @@
       <c r="O47" s="19"/>
     </row>
     <row r="48" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="28"/>
-      <c r="B48" s="21" t="s">
+      <c r="A48" s="27"/>
+      <c r="B48" s="18" t="s">
         <v>32</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D48" s="19" t="s">
         <v>11</v>
@@ -2673,12 +2676,12 @@
       <c r="O48" s="19"/>
     </row>
     <row r="49" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="18" t="s">
         <v>33</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D49" s="19" t="s">
         <v>11</v>
@@ -2696,12 +2699,12 @@
       <c r="O49" s="19"/>
     </row>
     <row r="50" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="28"/>
-      <c r="B50" s="18" t="s">
+      <c r="A50" s="27"/>
+      <c r="B50" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>11</v>
@@ -2719,48 +2722,50 @@
       <c r="O50" s="19"/>
     </row>
     <row r="51" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="28"/>
+      <c r="A51" s="28">
+        <v>2</v>
+      </c>
       <c r="B51" s="15" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
       <c r="E51" s="17">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F51" s="17">
-        <f t="shared" ref="F51:O51" si="15">E51</f>
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G51" s="17">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="H51" s="17">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="I51" s="17">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="J51" s="17">
-        <v>8</v>
+        <f t="shared" ref="J51:O51" si="22">I51</f>
+        <v>1</v>
       </c>
       <c r="K51" s="17">
         <v>0</v>
       </c>
       <c r="L51" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M51" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="N51" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="O51" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -2770,7 +2775,7 @@
         <v>30</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D52" s="19" t="s">
         <v>11</v>
@@ -2793,7 +2798,7 @@
         <v>31</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D53" s="19" t="s">
         <v>11</v>
@@ -2816,7 +2821,7 @@
         <v>32</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D54" s="19" t="s">
         <v>11</v>
@@ -2839,7 +2844,7 @@
         <v>33</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>11</v>
@@ -2862,7 +2867,7 @@
         <v>34</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D56" s="19" t="s">
         <v>11</v>
@@ -2879,53 +2884,49 @@
       <c r="N56" s="19"/>
       <c r="O56" s="19"/>
     </row>
-    <row r="57" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="28"/>
       <c r="B57" s="15" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C57" s="16"/>
       <c r="D57" s="16"/>
       <c r="E57" s="17">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="F57" s="17">
-        <f t="shared" ref="F57" si="16">E57</f>
-        <v>5</v>
+        <f t="shared" ref="F57:O57" si="23">E57</f>
+        <v>40</v>
       </c>
       <c r="G57" s="17">
-        <f t="shared" ref="G57" si="17">F57</f>
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="H57" s="17">
-        <f t="shared" ref="H57" si="18">G57</f>
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="I57" s="17">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J57" s="17">
-        <f t="shared" ref="J57" si="19">I57</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K57" s="17">
-        <f t="shared" ref="K57" si="20">J57</f>
         <v>0</v>
       </c>
       <c r="L57" s="17">
-        <f t="shared" ref="L57" si="21">K57</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="M57" s="17">
-        <f t="shared" ref="M57" si="22">L57</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="N57" s="17">
-        <f t="shared" ref="N57" si="23">M57</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O57" s="17">
-        <f t="shared" ref="O57" si="24">N57</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -2935,7 +2936,7 @@
         <v>30</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D58" s="19" t="s">
         <v>11</v>
@@ -2958,7 +2959,7 @@
         <v>31</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D59" s="19" t="s">
         <v>11</v>
@@ -2981,7 +2982,7 @@
         <v>32</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D60" s="19" t="s">
         <v>11</v>
@@ -3004,7 +3005,7 @@
         <v>33</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D61" s="19" t="s">
         <v>11</v>
@@ -3027,7 +3028,7 @@
         <v>34</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>11</v>
@@ -3047,50 +3048,50 @@
     <row r="63" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="28"/>
       <c r="B63" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C63" s="16"/>
       <c r="D63" s="16"/>
       <c r="E63" s="17">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F63" s="17">
-        <f t="shared" ref="F63" si="25">E63</f>
-        <v>8</v>
+        <f t="shared" ref="F63" si="24">E63</f>
+        <v>5</v>
       </c>
       <c r="G63" s="17">
-        <f t="shared" ref="G63" si="26">F63</f>
-        <v>8</v>
+        <f t="shared" ref="G63" si="25">F63</f>
+        <v>5</v>
       </c>
       <c r="H63" s="17">
-        <f t="shared" ref="H63" si="27">G63</f>
-        <v>8</v>
+        <f t="shared" ref="H63" si="26">G63</f>
+        <v>5</v>
       </c>
       <c r="I63" s="17">
-        <f t="shared" ref="I63" si="28">H63</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J63" s="17">
+        <f t="shared" ref="J63" si="27">I63</f>
         <v>0</v>
       </c>
       <c r="K63" s="17">
-        <f t="shared" ref="K63" si="29">J63</f>
+        <f t="shared" ref="K63" si="28">J63</f>
         <v>0</v>
       </c>
       <c r="L63" s="17">
-        <f t="shared" ref="L63" si="30">K63</f>
+        <f t="shared" ref="L63" si="29">K63</f>
         <v>0</v>
       </c>
       <c r="M63" s="17">
-        <f t="shared" ref="M63" si="31">L63</f>
+        <f t="shared" ref="M63" si="30">L63</f>
         <v>0</v>
       </c>
       <c r="N63" s="17">
-        <f t="shared" ref="N63" si="32">M63</f>
+        <f t="shared" ref="N63" si="31">M63</f>
         <v>0</v>
       </c>
       <c r="O63" s="17">
-        <f t="shared" ref="O63" si="33">N63</f>
+        <f t="shared" ref="O63" si="32">N63</f>
         <v>0</v>
       </c>
     </row>
@@ -3212,51 +3213,50 @@
     <row r="69" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="28"/>
       <c r="B69" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
       <c r="E69" s="17">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F69" s="17">
-        <f t="shared" ref="F69" si="34">E69</f>
-        <v>0</v>
+        <f t="shared" ref="F69" si="33">E69</f>
+        <v>8</v>
       </c>
       <c r="G69" s="17">
-        <f t="shared" ref="G69" si="35">F69</f>
-        <v>0</v>
+        <f t="shared" ref="G69" si="34">F69</f>
+        <v>8</v>
       </c>
       <c r="H69" s="17">
-        <f t="shared" ref="H69" si="36">G69</f>
-        <v>0</v>
+        <f t="shared" ref="H69" si="35">G69</f>
+        <v>8</v>
       </c>
       <c r="I69" s="17">
-        <f t="shared" ref="I69" si="37">H69</f>
-        <v>0</v>
+        <f t="shared" ref="I69" si="36">H69</f>
+        <v>8</v>
       </c>
       <c r="J69" s="17">
-        <f t="shared" ref="J69" si="38">I69</f>
         <v>0</v>
       </c>
       <c r="K69" s="17">
-        <f t="shared" ref="K69" si="39">J69</f>
+        <f t="shared" ref="K69" si="37">J69</f>
         <v>0</v>
       </c>
       <c r="L69" s="17">
-        <f t="shared" ref="L69" si="40">K69</f>
+        <f t="shared" ref="L69" si="38">K69</f>
         <v>0</v>
       </c>
       <c r="M69" s="17">
-        <f t="shared" ref="M69" si="41">L69</f>
+        <f t="shared" ref="M69" si="39">L69</f>
         <v>0</v>
       </c>
       <c r="N69" s="17">
-        <f t="shared" ref="N69" si="42">M69</f>
+        <f t="shared" ref="N69" si="40">M69</f>
         <v>0</v>
       </c>
       <c r="O69" s="17">
-        <f t="shared" ref="O69" si="43">N69</f>
+        <f t="shared" ref="O69" si="41">N69</f>
         <v>0</v>
       </c>
     </row>
@@ -3268,7 +3268,9 @@
       <c r="C70" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="19"/>
+      <c r="D70" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="E70" s="19"/>
       <c r="F70" s="19"/>
       <c r="G70" s="19"/>
@@ -3289,7 +3291,9 @@
       <c r="C71" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D71" s="19"/>
+      <c r="D71" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="E71" s="19"/>
       <c r="F71" s="19"/>
       <c r="G71" s="19"/>
@@ -3310,7 +3314,9 @@
       <c r="C72" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D72" s="19"/>
+      <c r="D72" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="E72" s="19"/>
       <c r="F72" s="19"/>
       <c r="G72" s="19"/>
@@ -3331,7 +3337,9 @@
       <c r="C73" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D73" s="19"/>
+      <c r="D73" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="E73" s="19"/>
       <c r="F73" s="19"/>
       <c r="G73" s="19"/>
@@ -3352,7 +3360,9 @@
       <c r="C74" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D74" s="19"/>
+      <c r="D74" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="E74" s="19"/>
       <c r="F74" s="19"/>
       <c r="G74" s="19"/>
@@ -3368,50 +3378,51 @@
     <row r="75" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="28"/>
       <c r="B75" s="15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C75" s="16"/>
       <c r="D75" s="16"/>
       <c r="E75" s="17">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F75" s="17">
-        <f t="shared" ref="F75" si="44">E75</f>
-        <v>9</v>
+        <f t="shared" ref="F75" si="42">E75</f>
+        <v>0</v>
       </c>
       <c r="G75" s="17">
-        <f t="shared" ref="G75" si="45">F75</f>
-        <v>9</v>
+        <f t="shared" ref="G75" si="43">F75</f>
+        <v>0</v>
       </c>
       <c r="H75" s="17">
-        <f t="shared" ref="H75" si="46">G75</f>
-        <v>9</v>
+        <f t="shared" ref="H75" si="44">G75</f>
+        <v>0</v>
       </c>
       <c r="I75" s="17">
-        <f t="shared" ref="I75" si="47">H75</f>
-        <v>9</v>
+        <f t="shared" ref="I75" si="45">H75</f>
+        <v>0</v>
       </c>
       <c r="J75" s="17">
-        <f t="shared" ref="J75" si="48">I75</f>
-        <v>9</v>
+        <f t="shared" ref="J75" si="46">I75</f>
+        <v>0</v>
       </c>
       <c r="K75" s="17">
+        <f t="shared" ref="K75" si="47">J75</f>
         <v>0</v>
       </c>
       <c r="L75" s="17">
-        <f t="shared" ref="L75" si="49">K75</f>
+        <f t="shared" ref="L75" si="48">K75</f>
         <v>0</v>
       </c>
       <c r="M75" s="17">
-        <f t="shared" ref="M75" si="50">L75</f>
+        <f t="shared" ref="M75" si="49">L75</f>
         <v>0</v>
       </c>
       <c r="N75" s="17">
-        <f t="shared" ref="N75" si="51">M75</f>
+        <f t="shared" ref="N75" si="50">M75</f>
         <v>0</v>
       </c>
       <c r="O75" s="17">
-        <f t="shared" ref="O75" si="52">N75</f>
+        <f t="shared" ref="O75" si="51">N75</f>
         <v>0</v>
       </c>
     </row>
@@ -3532,58 +3543,65 @@
     </row>
     <row r="81" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="28"/>
-      <c r="B81" s="15"/>
+      <c r="B81" s="15" t="s">
+        <v>49</v>
+      </c>
       <c r="C81" s="16"/>
       <c r="D81" s="16"/>
       <c r="E81" s="17">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F81" s="17">
-        <f t="shared" ref="F81:O81" si="53">E81</f>
-        <v>0</v>
+        <f t="shared" ref="F81" si="52">E81</f>
+        <v>9</v>
       </c>
       <c r="G81" s="17">
-        <f t="shared" si="53"/>
-        <v>0</v>
+        <f t="shared" ref="G81" si="53">F81</f>
+        <v>9</v>
       </c>
       <c r="H81" s="17">
-        <f t="shared" si="53"/>
-        <v>0</v>
+        <f t="shared" ref="H81" si="54">G81</f>
+        <v>9</v>
       </c>
       <c r="I81" s="17">
-        <f t="shared" si="53"/>
-        <v>0</v>
+        <f t="shared" ref="I81" si="55">H81</f>
+        <v>9</v>
       </c>
       <c r="J81" s="17">
-        <f t="shared" si="53"/>
-        <v>0</v>
+        <f t="shared" ref="J81" si="56">I81</f>
+        <v>9</v>
       </c>
       <c r="K81" s="17">
-        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="L81" s="17">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="L81" si="57">K81</f>
         <v>0</v>
       </c>
       <c r="M81" s="17">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="M81" si="58">L81</f>
         <v>0</v>
       </c>
       <c r="N81" s="17">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="N81" si="59">M81</f>
         <v>0</v>
       </c>
       <c r="O81" s="17">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="O81" si="60">N81</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="28"/>
-      <c r="B82" s="18"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
+      <c r="B82" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C82" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="E82" s="19"/>
       <c r="F82" s="19"/>
       <c r="G82" s="19"/>
@@ -3598,9 +3616,15 @@
     </row>
     <row r="83" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="28"/>
-      <c r="B83" s="18"/>
-      <c r="C83" s="19"/>
-      <c r="D83" s="19"/>
+      <c r="B83" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="E83" s="19"/>
       <c r="F83" s="19"/>
       <c r="G83" s="19"/>
@@ -3615,9 +3639,15 @@
     </row>
     <row r="84" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="28"/>
-      <c r="B84" s="18"/>
-      <c r="C84" s="19"/>
-      <c r="D84" s="19"/>
+      <c r="B84" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="E84" s="19"/>
       <c r="F84" s="19"/>
       <c r="G84" s="19"/>
@@ -3632,9 +3662,15 @@
     </row>
     <row r="85" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="28"/>
-      <c r="B85" s="18"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="19"/>
+      <c r="B85" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C85" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="E85" s="19"/>
       <c r="F85" s="19"/>
       <c r="G85" s="19"/>
@@ -3649,9 +3685,15 @@
     </row>
     <row r="86" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="28"/>
-      <c r="B86" s="18"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="19"/>
+      <c r="B86" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C86" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="E86" s="19"/>
       <c r="F86" s="19"/>
       <c r="G86" s="19"/>
@@ -3664,67 +3706,60 @@
       <c r="N86" s="19"/>
       <c r="O86" s="19"/>
     </row>
-    <row r="87" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="28"/>
-      <c r="B87" s="15" t="s">
-        <v>44</v>
-      </c>
+      <c r="B87" s="15"/>
       <c r="C87" s="16"/>
       <c r="D87" s="16"/>
       <c r="E87" s="17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F87" s="17">
-        <f t="shared" ref="F87" si="54">E87</f>
-        <v>5</v>
+        <f t="shared" ref="F87:O87" si="61">E87</f>
+        <v>0</v>
       </c>
       <c r="G87" s="17">
-        <f t="shared" ref="G87" si="55">F87</f>
-        <v>5</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="H87" s="17">
-        <f t="shared" ref="H87" si="56">G87</f>
-        <v>5</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="I87" s="17">
-        <f t="shared" ref="I87" si="57">H87</f>
-        <v>5</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="J87" s="17">
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="K87" s="17">
-        <f t="shared" ref="K87" si="58">J87</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="L87" s="17">
-        <f t="shared" ref="L87" si="59">K87</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="M87" s="17">
-        <f t="shared" ref="M87" si="60">L87</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="N87" s="17">
-        <f t="shared" ref="N87" si="61">M87</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="O87" s="17">
-        <f t="shared" ref="O87" si="62">N87</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="28"/>
-      <c r="B88" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C88" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D88" s="19" t="s">
-        <v>11</v>
-      </c>
+      <c r="B88" s="18"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
       <c r="E88" s="19"/>
       <c r="F88" s="19"/>
       <c r="G88" s="19"/>
@@ -3739,15 +3774,9 @@
     </row>
     <row r="89" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="28"/>
-      <c r="B89" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C89" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D89" s="19" t="s">
-        <v>11</v>
-      </c>
+      <c r="B89" s="18"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
       <c r="E89" s="19"/>
       <c r="F89" s="19"/>
       <c r="G89" s="19"/>
@@ -3762,15 +3791,9 @@
     </row>
     <row r="90" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="28"/>
-      <c r="B90" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C90" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D90" s="19" t="s">
-        <v>11</v>
-      </c>
+      <c r="B90" s="18"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="19"/>
       <c r="E90" s="19"/>
       <c r="F90" s="19"/>
       <c r="G90" s="19"/>
@@ -3785,15 +3808,9 @@
     </row>
     <row r="91" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="28"/>
-      <c r="B91" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C91" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" s="19" t="s">
-        <v>11</v>
-      </c>
+      <c r="B91" s="18"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="19"/>
       <c r="E91" s="19"/>
       <c r="F91" s="19"/>
       <c r="G91" s="19"/>
@@ -3808,15 +3825,9 @@
     </row>
     <row r="92" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="28"/>
-      <c r="B92" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C92" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D92" s="19" t="s">
-        <v>11</v>
-      </c>
+      <c r="B92" s="18"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
       <c r="E92" s="19"/>
       <c r="F92" s="19"/>
       <c r="G92" s="19"/>
@@ -3832,50 +3843,51 @@
     <row r="93" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A93" s="28"/>
       <c r="B93" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C93" s="16"/>
       <c r="D93" s="16"/>
       <c r="E93" s="17">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F93" s="17">
-        <f t="shared" ref="F93" si="63">E93</f>
-        <v>10</v>
+        <f t="shared" ref="F93" si="62">E93</f>
+        <v>5</v>
       </c>
       <c r="G93" s="17">
-        <f t="shared" ref="G93" si="64">F93</f>
-        <v>10</v>
+        <f t="shared" ref="G93" si="63">F93</f>
+        <v>5</v>
       </c>
       <c r="H93" s="17">
-        <f t="shared" ref="H93" si="65">G93</f>
-        <v>10</v>
+        <f t="shared" ref="H93" si="64">G93</f>
+        <v>5</v>
       </c>
       <c r="I93" s="17">
-        <f t="shared" ref="I93" si="66">H93</f>
-        <v>10</v>
+        <f t="shared" ref="I93" si="65">H93</f>
+        <v>5</v>
       </c>
       <c r="J93" s="17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K93" s="17">
-        <v>4</v>
+        <f t="shared" ref="K93" si="66">J93</f>
+        <v>0</v>
       </c>
       <c r="L93" s="17">
         <f t="shared" ref="L93" si="67">K93</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M93" s="17">
         <f t="shared" ref="M93" si="68">L93</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N93" s="17">
         <f t="shared" ref="N93" si="69">M93</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O93" s="17">
         <f t="shared" ref="O93" si="70">N93</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3884,10 +3896,10 @@
         <v>30</v>
       </c>
       <c r="C94" s="19" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D94" s="19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E94" s="19"/>
       <c r="F94" s="19"/>
@@ -3907,10 +3919,10 @@
         <v>31</v>
       </c>
       <c r="C95" s="19" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D95" s="19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E95" s="19"/>
       <c r="F95" s="19"/>
@@ -3930,10 +3942,10 @@
         <v>32</v>
       </c>
       <c r="C96" s="19" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D96" s="19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E96" s="19"/>
       <c r="F96" s="19"/>
@@ -3953,10 +3965,10 @@
         <v>33</v>
       </c>
       <c r="C97" s="19" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D97" s="19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E97" s="19"/>
       <c r="F97" s="19"/>
@@ -3976,10 +3988,10 @@
         <v>34</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D98" s="19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E98" s="19"/>
       <c r="F98" s="19"/>
@@ -3996,50 +4008,48 @@
     <row r="99" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A99" s="28"/>
       <c r="B99" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C99" s="16"/>
       <c r="D99" s="16"/>
       <c r="E99" s="17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F99" s="17">
         <f t="shared" ref="F99" si="71">E99</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G99" s="17">
         <f t="shared" ref="G99" si="72">F99</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H99" s="17">
         <f t="shared" ref="H99" si="73">G99</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I99" s="17">
         <f t="shared" ref="I99" si="74">H99</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J99" s="17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K99" s="17">
-        <f t="shared" ref="K99" si="75">J99</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L99" s="17">
-        <f t="shared" ref="L99" si="76">K99</f>
-        <v>0</v>
+        <f t="shared" ref="L99" si="75">K99</f>
+        <v>4</v>
       </c>
       <c r="M99" s="17">
-        <f t="shared" ref="M99" si="77">L99</f>
-        <v>0</v>
+        <f t="shared" ref="M99" si="76">L99</f>
+        <v>4</v>
       </c>
       <c r="N99" s="17">
-        <f t="shared" ref="N99" si="78">M99</f>
         <v>0</v>
       </c>
       <c r="O99" s="17">
-        <f t="shared" ref="O99" si="79">N99</f>
+        <f t="shared" ref="O99" si="77">N99</f>
         <v>0</v>
       </c>
     </row>
@@ -4158,28 +4168,67 @@
       <c r="N104" s="19"/>
       <c r="O104" s="19"/>
     </row>
-    <row r="105" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A105" s="28"/>
-      <c r="B105" s="18"/>
-      <c r="C105" s="19"/>
-      <c r="D105" s="19"/>
-      <c r="E105" s="19"/>
-      <c r="F105" s="19"/>
-      <c r="G105" s="19"/>
-      <c r="H105" s="19"/>
-      <c r="I105" s="19"/>
-      <c r="J105" s="19"/>
-      <c r="K105" s="19"/>
-      <c r="L105" s="19"/>
-      <c r="M105" s="19"/>
-      <c r="N105" s="19"/>
-      <c r="O105" s="19"/>
+      <c r="B105" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C105" s="16"/>
+      <c r="D105" s="16"/>
+      <c r="E105" s="17">
+        <v>5</v>
+      </c>
+      <c r="F105" s="17">
+        <f t="shared" ref="F105" si="78">E105</f>
+        <v>5</v>
+      </c>
+      <c r="G105" s="17">
+        <f t="shared" ref="G105" si="79">F105</f>
+        <v>5</v>
+      </c>
+      <c r="H105" s="17">
+        <f t="shared" ref="H105" si="80">G105</f>
+        <v>5</v>
+      </c>
+      <c r="I105" s="17">
+        <f t="shared" ref="I105" si="81">H105</f>
+        <v>5</v>
+      </c>
+      <c r="J105" s="17">
+        <v>0</v>
+      </c>
+      <c r="K105" s="17">
+        <f t="shared" ref="K105" si="82">J105</f>
+        <v>0</v>
+      </c>
+      <c r="L105" s="17">
+        <f t="shared" ref="L105" si="83">K105</f>
+        <v>0</v>
+      </c>
+      <c r="M105" s="17">
+        <f t="shared" ref="M105" si="84">L105</f>
+        <v>0</v>
+      </c>
+      <c r="N105" s="17">
+        <f t="shared" ref="N105" si="85">M105</f>
+        <v>0</v>
+      </c>
+      <c r="O105" s="17">
+        <f t="shared" ref="O105" si="86">N105</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="106" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="28"/>
-      <c r="B106" s="18"/>
-      <c r="C106" s="19"/>
-      <c r="D106" s="19"/>
+      <c r="B106" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C106" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D106" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="E106" s="19"/>
       <c r="F106" s="19"/>
       <c r="G106" s="19"/>
@@ -4192,105 +4241,231 @@
       <c r="N106" s="19"/>
       <c r="O106" s="19"/>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B107" s="22" t="s">
+    <row r="107" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="28"/>
+      <c r="B107" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C107" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D107" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E107" s="19"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="19"/>
+      <c r="H107" s="19"/>
+      <c r="I107" s="19"/>
+      <c r="J107" s="19"/>
+      <c r="K107" s="19"/>
+      <c r="L107" s="19"/>
+      <c r="M107" s="19"/>
+      <c r="N107" s="19"/>
+      <c r="O107" s="19"/>
+    </row>
+    <row r="108" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="28"/>
+      <c r="B108" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C108" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E108" s="19"/>
+      <c r="F108" s="19"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="19"/>
+      <c r="I108" s="19"/>
+      <c r="J108" s="19"/>
+      <c r="K108" s="19"/>
+      <c r="L108" s="19"/>
+      <c r="M108" s="19"/>
+      <c r="N108" s="19"/>
+      <c r="O108" s="19"/>
+    </row>
+    <row r="109" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="28"/>
+      <c r="B109" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C109" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D109" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E109" s="19"/>
+      <c r="F109" s="19"/>
+      <c r="G109" s="19"/>
+      <c r="H109" s="19"/>
+      <c r="I109" s="19"/>
+      <c r="J109" s="19"/>
+      <c r="K109" s="19"/>
+      <c r="L109" s="19"/>
+      <c r="M109" s="19"/>
+      <c r="N109" s="19"/>
+      <c r="O109" s="19"/>
+    </row>
+    <row r="110" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="28"/>
+      <c r="B110" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C110" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D110" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="19"/>
+      <c r="H110" s="19"/>
+      <c r="I110" s="19"/>
+      <c r="J110" s="19"/>
+      <c r="K110" s="19"/>
+      <c r="L110" s="19"/>
+      <c r="M110" s="19"/>
+      <c r="N110" s="19"/>
+      <c r="O110" s="19"/>
+    </row>
+    <row r="111" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="28"/>
+      <c r="B111" s="18"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="19"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="19"/>
+      <c r="H111" s="19"/>
+      <c r="I111" s="19"/>
+      <c r="J111" s="19"/>
+      <c r="K111" s="19"/>
+      <c r="L111" s="19"/>
+      <c r="M111" s="19"/>
+      <c r="N111" s="19"/>
+      <c r="O111" s="19"/>
+    </row>
+    <row r="112" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="28"/>
+      <c r="B112" s="18"/>
+      <c r="C112" s="19"/>
+      <c r="D112" s="19"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="19"/>
+      <c r="G112" s="19"/>
+      <c r="H112" s="19"/>
+      <c r="I112" s="19"/>
+      <c r="J112" s="19"/>
+      <c r="K112" s="19"/>
+      <c r="L112" s="19"/>
+      <c r="M112" s="19"/>
+      <c r="N112" s="19"/>
+      <c r="O112" s="19"/>
+    </row>
+    <row r="113" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B113" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C107" s="22"/>
-      <c r="D107" s="22"/>
-      <c r="E107" s="22">
-        <f t="shared" ref="E107:O107" si="80">SUM(E7:E106)</f>
-        <v>162</v>
-      </c>
-      <c r="F107" s="22">
-        <f t="shared" si="80"/>
-        <v>143</v>
-      </c>
-      <c r="G107" s="22">
-        <f t="shared" si="80"/>
-        <v>119</v>
-      </c>
-      <c r="H107" s="22">
-        <f t="shared" si="80"/>
-        <v>103</v>
-      </c>
-      <c r="I107" s="22">
-        <f t="shared" si="80"/>
-        <v>73</v>
-      </c>
-      <c r="J107" s="22">
-        <f t="shared" si="80"/>
-        <v>39</v>
-      </c>
-      <c r="K107" s="22">
-        <f t="shared" si="80"/>
-        <v>12</v>
-      </c>
-      <c r="L107" s="22">
-        <f t="shared" si="80"/>
-        <v>12</v>
-      </c>
-      <c r="M107" s="22">
-        <f t="shared" si="80"/>
-        <v>12</v>
-      </c>
-      <c r="N107" s="22">
-        <f t="shared" si="80"/>
-        <v>12</v>
-      </c>
-      <c r="O107" s="22">
-        <f t="shared" si="80"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B108" s="22" t="s">
+      <c r="C113" s="22"/>
+      <c r="D113" s="22"/>
+      <c r="E113" s="22">
+        <f t="shared" ref="E113:O113" si="87">SUM(E7:E112)</f>
+        <v>168</v>
+      </c>
+      <c r="F113" s="22">
+        <f t="shared" si="87"/>
+        <v>149</v>
+      </c>
+      <c r="G113" s="22">
+        <f t="shared" si="87"/>
+        <v>125</v>
+      </c>
+      <c r="H113" s="22">
+        <f t="shared" si="87"/>
+        <v>109</v>
+      </c>
+      <c r="I113" s="22">
+        <f t="shared" si="87"/>
+        <v>74</v>
+      </c>
+      <c r="J113" s="22">
+        <f t="shared" si="87"/>
+        <v>40</v>
+      </c>
+      <c r="K113" s="22">
+        <f t="shared" si="87"/>
+        <v>13</v>
+      </c>
+      <c r="L113" s="22">
+        <f t="shared" si="87"/>
+        <v>13</v>
+      </c>
+      <c r="M113" s="22">
+        <f t="shared" si="87"/>
+        <v>6</v>
+      </c>
+      <c r="N113" s="22">
+        <f t="shared" si="87"/>
+        <v>1</v>
+      </c>
+      <c r="O113" s="22">
+        <f t="shared" si="87"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B114" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C108" s="22"/>
-      <c r="D108" s="22"/>
-      <c r="E108" s="22">
+      <c r="C114" s="22"/>
+      <c r="D114" s="22"/>
+      <c r="E114" s="22">
         <f>Paramètres!D2*Paramètres!D4*COLUMNS(F6:O6)</f>
         <v>70</v>
       </c>
-      <c r="F108" s="22">
-        <f>E108-(Paramètres!$D2*Paramètres!$D4)</f>
+      <c r="F114" s="22">
+        <f>E114-(Paramètres!$D2*Paramètres!$D4)</f>
         <v>63</v>
       </c>
-      <c r="G108" s="22">
-        <f>F108-(Paramètres!$D2*Paramètres!$D4)</f>
+      <c r="G114" s="22">
+        <f>F114-(Paramètres!$D2*Paramètres!$D4)</f>
         <v>56</v>
       </c>
-      <c r="H108" s="22">
-        <f>G108-(Paramètres!$D2*Paramètres!$D4)</f>
+      <c r="H114" s="22">
+        <f>G114-(Paramètres!$D2*Paramètres!$D4)</f>
         <v>49</v>
       </c>
-      <c r="I108" s="22">
-        <f>H108-(Paramètres!$D2*Paramètres!$D4)</f>
+      <c r="I114" s="22">
+        <f>H114-(Paramètres!$D2*Paramètres!$D4)</f>
         <v>42</v>
       </c>
-      <c r="J108" s="22">
-        <f>I108-(Paramètres!$D2*Paramètres!$D4)</f>
+      <c r="J114" s="22">
+        <f>I114-(Paramètres!$D2*Paramètres!$D4)</f>
         <v>35</v>
       </c>
-      <c r="K108" s="22">
-        <f>J108-(Paramètres!$D2*Paramètres!$D4)</f>
+      <c r="K114" s="22">
+        <f>J114-(Paramètres!$D2*Paramètres!$D4)</f>
         <v>28</v>
       </c>
-      <c r="L108" s="22">
-        <f>K108-(Paramètres!$D2*Paramètres!$D4)</f>
+      <c r="L114" s="22">
+        <f>K114-(Paramètres!$D2*Paramètres!$D4)</f>
         <v>21</v>
       </c>
-      <c r="M108" s="22">
-        <f>L108-(Paramètres!$D2*Paramètres!$D4)</f>
+      <c r="M114" s="22">
+        <f>L114-(Paramètres!$D2*Paramètres!$D4)</f>
         <v>14</v>
       </c>
-      <c r="N108" s="22">
-        <f>M108-(Paramètres!$D2*Paramètres!$D4)</f>
+      <c r="N114" s="22">
+        <f>M114-(Paramètres!$D2*Paramètres!$D4)</f>
         <v>7</v>
       </c>
-      <c r="O108" s="22">
-        <f>N108-(Paramètres!$D2*Paramètres!$D4)</f>
+      <c r="O114" s="22">
+        <f>N114-(Paramètres!$D2*Paramètres!$D4)</f>
         <v>0</v>
       </c>
     </row>
@@ -4298,8 +4473,8 @@
   <mergeCells count="4">
     <mergeCell ref="A3:P3"/>
     <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A15:A44"/>
-    <mergeCell ref="A45:A106"/>
+    <mergeCell ref="A15:A50"/>
+    <mergeCell ref="A51:A112"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4310,13 +4485,13 @@
           <x14:formula1>
             <xm:f>Paramètres!$C$5:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C7:C106</xm:sqref>
+          <xm:sqref>C7:C112</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Paramètres!$C$11:$C$14</xm:f>
           </x14:formula1>
-          <xm:sqref>D7:D106</xm:sqref>
+          <xm:sqref>D7:D112</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>